<commit_message>
finished organizing existing code
</commit_message>
<xml_diff>
--- a/COV_EST_TIMELINE.xlsx
+++ b/COV_EST_TIMELINE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intlmonetaryfund-my.sharepoint.com/personal/mxiao_imf_org1/Documents/COV_EST/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="11_F25DC773A252ABDACC1048DEE159726C5BDE58FE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D23451FD-C9F5-4FEB-A86B-D3DEF5FF2A28}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="11_F25DC773A252ABDACC1048DEE159726C5BDE58FE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FABD1803-5294-4302-9E9B-6E9E0E3619FF}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$8</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -215,6 +216,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>

</xml_diff>